<commit_message>
Good updated for condenser
</commit_message>
<xml_diff>
--- a/DiscreteEvaporator/InputDoc/CondStruc.xlsx
+++ b/DiscreteEvaporator/InputDoc/CondStruc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10260" yWindow="1820" windowWidth="28720" windowHeight="17620" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="16600" yWindow="3380" windowWidth="28720" windowHeight="17620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="description" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>air flow rate [m^3/s]</t>
   </si>
   <si>
-    <t>EvapStruc</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>RowNo</t>
   </si>
   <si>
-    <t>Refdownstream</t>
-  </si>
-  <si>
     <t>AirUpstreamUpper</t>
   </si>
   <si>
@@ -99,6 +93,12 @@
   </si>
   <si>
     <t>tube number (total)</t>
+  </si>
+  <si>
+    <t>CondStruc</t>
+  </si>
+  <si>
+    <t>RefUpstream</t>
   </si>
 </sst>
 </file>
@@ -474,18 +474,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -501,7 +499,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -517,7 +515,7 @@
         <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -599,23 +597,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -666,11 +664,46 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -689,16 +722,16 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
@@ -911,8 +944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:A51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -923,25 +956,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>